<commit_message>
make some changes Signed-off-by: 赵成明 <zhaochengming@meituan.com>
</commit_message>
<xml_diff>
--- a/Morvan/02_Q_Learning_maze/qlearn_log.xlsx
+++ b/Morvan/02_Q_Learning_maze/qlearn_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="5">
   <si>
     <t>episode</t>
   </si>
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -408,7 +408,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -419,7 +419,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -430,10 +430,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -441,10 +441,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -463,10 +463,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -474,7 +474,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -485,10 +485,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -496,10 +496,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -507,7 +507,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -518,7 +518,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -529,7 +529,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -540,10 +540,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -551,7 +551,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -562,7 +562,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -584,7 +584,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -595,7 +595,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -606,7 +606,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -639,7 +639,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -650,7 +650,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -694,7 +694,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -749,7 +749,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -760,7 +760,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -771,7 +771,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -804,7 +804,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
@@ -815,7 +815,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
@@ -826,10 +826,10 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -837,7 +837,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -848,10 +848,10 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -881,7 +881,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C45" t="s">
         <v>4</v>
@@ -903,7 +903,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s">
         <v>4</v>
@@ -914,10 +914,10 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -925,7 +925,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C49" t="s">
         <v>4</v>
@@ -936,7 +936,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C50" t="s">
         <v>4</v>
@@ -951,556 +951,6 @@
       </c>
       <c r="C51" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="B53">
-        <v>6</v>
-      </c>
-      <c r="C53" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="B54">
-        <v>3</v>
-      </c>
-      <c r="C54" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55">
-        <v>8</v>
-      </c>
-      <c r="C55" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56">
-        <v>7</v>
-      </c>
-      <c r="C56" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="B57">
-        <v>6</v>
-      </c>
-      <c r="C57" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58">
-        <v>7</v>
-      </c>
-      <c r="C58" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59">
-        <v>6</v>
-      </c>
-      <c r="C59" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="B60">
-        <v>8</v>
-      </c>
-      <c r="C60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61">
-        <v>7</v>
-      </c>
-      <c r="C61" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62">
-        <v>8</v>
-      </c>
-      <c r="C62" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63">
-        <v>11</v>
-      </c>
-      <c r="C63" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64">
-        <v>63</v>
-      </c>
-      <c r="B64">
-        <v>8</v>
-      </c>
-      <c r="C64" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="B65">
-        <v>6</v>
-      </c>
-      <c r="C65" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66">
-        <v>65</v>
-      </c>
-      <c r="B66">
-        <v>6</v>
-      </c>
-      <c r="C66" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="B67">
-        <v>6</v>
-      </c>
-      <c r="C67" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="B68">
-        <v>6</v>
-      </c>
-      <c r="C68" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69">
-        <v>68</v>
-      </c>
-      <c r="B69">
-        <v>6</v>
-      </c>
-      <c r="C69" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70">
-        <v>69</v>
-      </c>
-      <c r="B70">
-        <v>6</v>
-      </c>
-      <c r="C70" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="B71">
-        <v>6</v>
-      </c>
-      <c r="C71" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72">
-        <v>71</v>
-      </c>
-      <c r="B72">
-        <v>6</v>
-      </c>
-      <c r="C72" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="B73">
-        <v>7</v>
-      </c>
-      <c r="C73" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="B74">
-        <v>6</v>
-      </c>
-      <c r="C74" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75">
-        <v>74</v>
-      </c>
-      <c r="B75">
-        <v>6</v>
-      </c>
-      <c r="C75" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76">
-        <v>75</v>
-      </c>
-      <c r="B76">
-        <v>3</v>
-      </c>
-      <c r="C76" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="B77">
-        <v>6</v>
-      </c>
-      <c r="C77" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78">
-        <v>8</v>
-      </c>
-      <c r="C78" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="B79">
-        <v>10</v>
-      </c>
-      <c r="C79" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80">
-        <v>79</v>
-      </c>
-      <c r="B80">
-        <v>6</v>
-      </c>
-      <c r="C80" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81">
-        <v>80</v>
-      </c>
-      <c r="B81">
-        <v>6</v>
-      </c>
-      <c r="C81" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82">
-        <v>81</v>
-      </c>
-      <c r="B82">
-        <v>6</v>
-      </c>
-      <c r="C82" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83">
-        <v>82</v>
-      </c>
-      <c r="B83">
-        <v>6</v>
-      </c>
-      <c r="C83" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84">
-        <v>83</v>
-      </c>
-      <c r="B84">
-        <v>10</v>
-      </c>
-      <c r="C84" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85">
-        <v>84</v>
-      </c>
-      <c r="B85">
-        <v>7</v>
-      </c>
-      <c r="C85" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86">
-        <v>85</v>
-      </c>
-      <c r="B86">
-        <v>6</v>
-      </c>
-      <c r="C86" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87">
-        <v>86</v>
-      </c>
-      <c r="B87">
-        <v>10</v>
-      </c>
-      <c r="C87" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88">
-        <v>87</v>
-      </c>
-      <c r="B88">
-        <v>6</v>
-      </c>
-      <c r="C88" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89">
-        <v>88</v>
-      </c>
-      <c r="B89">
-        <v>7</v>
-      </c>
-      <c r="C89" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90">
-        <v>89</v>
-      </c>
-      <c r="B90">
-        <v>6</v>
-      </c>
-      <c r="C90" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91">
-        <v>90</v>
-      </c>
-      <c r="B91">
-        <v>7</v>
-      </c>
-      <c r="C91" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92">
-        <v>91</v>
-      </c>
-      <c r="B92">
-        <v>3</v>
-      </c>
-      <c r="C92" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93">
-        <v>92</v>
-      </c>
-      <c r="B93">
-        <v>6</v>
-      </c>
-      <c r="C93" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94">
-        <v>93</v>
-      </c>
-      <c r="B94">
-        <v>7</v>
-      </c>
-      <c r="C94" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95">
-        <v>94</v>
-      </c>
-      <c r="B95">
-        <v>10</v>
-      </c>
-      <c r="C95" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="A96">
-        <v>95</v>
-      </c>
-      <c r="B96">
-        <v>6</v>
-      </c>
-      <c r="C96" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97">
-        <v>96</v>
-      </c>
-      <c r="B97">
-        <v>8</v>
-      </c>
-      <c r="C97" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98">
-        <v>97</v>
-      </c>
-      <c r="B98">
-        <v>6</v>
-      </c>
-      <c r="C98" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99">
-        <v>98</v>
-      </c>
-      <c r="B99">
-        <v>6</v>
-      </c>
-      <c r="C99" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100">
-        <v>99</v>
-      </c>
-      <c r="B100">
-        <v>6</v>
-      </c>
-      <c r="C100" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101">
-        <v>100</v>
-      </c>
-      <c r="B101">
-        <v>5</v>
-      </c>
-      <c r="C101" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>